<commit_message>
adding data into input sheet
</commit_message>
<xml_diff>
--- a/InputExcelSheet/Input_parameterization123.xlsx
+++ b/InputExcelSheet/Input_parameterization123.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
   <si>
     <t xml:space="preserve">Feature Name</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">DELETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provider</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFFFF00"/>
       <name val="Bahnschrift SemiLight"/>
       <family val="2"/>
       <charset val="1"/>
@@ -141,8 +144,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFF9900"/>
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
@@ -298,7 +301,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFBF00"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
@@ -321,10 +324,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -485,6 +488,54 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
     </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>